<commit_message>
WIP: brother_toners. fixing excel writing placement
</commit_message>
<xml_diff>
--- a/Brother.xlsx
+++ b/Brother.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BrotherModels" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="BrotherToners" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="963">
   <si>
     <t>dcp-1000</t>
   </si>
@@ -2622,24 +2623,12 @@
     <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j870dw</t>
   </si>
   <si>
-    <t>mfc-j870dw-650</t>
-  </si>
-  <si>
-    <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j870dw-650</t>
-  </si>
-  <si>
     <t>mfc-j875dw</t>
   </si>
   <si>
     <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j875dw</t>
   </si>
   <si>
-    <t>mfc-j875dw-650</t>
-  </si>
-  <si>
-    <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j875dw-650</t>
-  </si>
-  <si>
     <t>mfcl2680w</t>
   </si>
   <si>
@@ -2782,12 +2771,162 @@
   </si>
   <si>
     <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/ppf/ppf-580mc</t>
+  </si>
+  <si>
+    <t>Genuine Brother cyan toner for HL4040cn, HL4040cdn, HL4070cdw, MFC9440cn, MFC9450cdn, MFC9840cdw, DCP9040cn, DCP9045cdn. A cartridge that will perform when your requirements are most demanding. Each cartridge produces solid blacks and vibrant colors for eye-catching graphics. Increase productivity and reduce costs when each cartridge delivers value and dependability.</t>
+  </si>
+  <si>
+    <t>Genuine Brother magenta toner for HL4040cn, HL4040cdn, HL4070cdw, MFC9440cn, MFC9450cdn, MFC9840cdw, DCP9040cn, DCP9045cdn. A cartridge that will perform when your requirements are most demanding. Each cartridge produces solid blacks and vibrant colors for eye-catching graphics. Increase productivity and reduce costs when each cartridge delivers value and dependability.</t>
+  </si>
+  <si>
+    <t>Genuine Brother black toner for HL4040cn, HL4040cdn, HL4070cdw, MFC9440cn, MFC9450cdn, MFC9840cdw, DCP9040cn, DCP9045cdn. A cartridge that will perform when your requirements are most demanding. Each cartridge produces solid blacks and vibrant colors for eye-catching graphics. Increase productivity and reduce costs when each cartridge delivers value and dependability.</t>
+  </si>
+  <si>
+    <t>Genuine Brother toner value pack for HL4040cn, HL4040cdn, HL4070cdw, MFC9440cn, MFC9450cdn, MFC9840cdw, DCP9040cn, DCP9045cdn. Value Pack includes one of each color.  Black TN115BK, cyan TN115C, magenta TN115M, and yellow TN115Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine Brother cyan toner for DCP9010cn, HL3040cn, HL3045cn, HL3070cw, HL3075, HL3075cw, MFC9010cn, MFC9120cn, MFC9125CN, MFC9320cn, MFC9325cn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine Brother magenta toner for DCP9010cn, HL3040cn, HL3045cn, HL3070cw, HL3075, HL3075cw, MFC9010cn, MFC9120cn, MFC9125CN, MFC9320cn, MFC9325cn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium compatible high-yield toner for DCP-L5500DN, DCP-L5600DN, DCP-L5650DN, HL-L5000D, HL-L5100DN, HL-L5200, HL-L6200, HL-L6250DW, HL-L6300DW, HL-L6400DW, MFC-L5700DW, MDC-L5800DW, MFC-L5850DW, MFC-L5900DW, MFC-L6750DW, MFC-L6800DW. </t>
+  </si>
+  <si>
+    <t>Genuine Brother toner value pack for use in HL4040cn, HL4040cdn, HL4070cdw, MFC9440cn, MFC9450cdn, MFC9840cdw, DCP9040cn, DCP9045cdn.</t>
+  </si>
+  <si>
+    <t>Premium compatible high-yield magenta toner for HL-L8260CDW, HL-L8360CDW, HL-L8360CDWT, MFC-L8610CDW, MFC-L8900CDW.</t>
+  </si>
+  <si>
+    <t>Premium compatible high-yield cyan toner for HL-L8260CDW, HL-L8360CDW, HL-L8360CDWT, MFC-L8610CDW, MFC-L8900CDW.</t>
+  </si>
+  <si>
+    <t>Genuine Brother cyan toner for HL-L8260CDW, HL-L8360CDW, HL-L8360CDWT, MFC-L8610CDW, MFC-L8900CDW.</t>
+  </si>
+  <si>
+    <t>Premium compatible high-yield black toner for HL-L8260CDW, HL-L8360CDW, HL-L8360CDWT, MFC-L8610CDW, MFC-L8900CDW.</t>
+  </si>
+  <si>
+    <t>Genuine Brother high-yield black toner for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw.</t>
+  </si>
+  <si>
+    <t>Genuine Brother magenta toner for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw.</t>
+  </si>
+  <si>
+    <t>Genuine Brother cyan toner for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw.</t>
+  </si>
+  <si>
+    <t>Genuine Brother high-yield toner value pack for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw. Contains one of each color. Black TN336BK, cyan TN336C, magenta TN366M, yellow TN336Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium compatible high-yield yellow toner for Brother HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw. </t>
+  </si>
+  <si>
+    <t>Genuine Brother black toner for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium compatible high-yield black toner for Brother HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw. </t>
+  </si>
+  <si>
+    <t>Premium compatible high-yield toner value pack for HL-L8260CDW, HL-L8360CDW, HL-L8360CDWT, MFC-L8610CDW, MFC-L8900CDW. Contains one of each color. Black TN433BK, Cyan TN433C, Magenta TN433M, Yellow TN433Y.</t>
+  </si>
+  <si>
+    <t>Premium compatible high-yield toner value pack for Brother HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw. Contains one of each color. Black TN336BK, cyan TN336C, magenta TN366M, yellow TN336Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine Brother super high-yield toner for HL-L6200DW, HL-L6250DW, HL-L6200DWT, HL-L6300DW, HL-L6400DWT, HL-L6400DW, HL-L6400DWT, MFC-L5700, MFC-L6700DW, MFC-L6750DW, MFC-L6800DW. </t>
+  </si>
+  <si>
+    <t>Genuine Brother yellow toner for HL-L8250cdn, HL-L8350cdw, HL-L8350cdwt, MFC-L8600cdw, MFC-L8850cdw.</t>
+  </si>
+  <si>
+    <t>Premium compatible toner for Brother HL-L6400DW, HL-L6400DWT, HL-L6900DW, MFC-L6900DW.</t>
+  </si>
+  <si>
+    <t>Premium compatible super high-yield toner for Brother HL-L6200DW, HL-L6250DW, HL-L6200DWT, HL-L6300DW, HL-L6400DWT, HL-L6400DW, HL-L6400DWT, MFC-L5700, MFC-L6700DW, MFC-L6750DW, MFC-L6800DW. Contains 3 compatible high-yield black toner cartridges.</t>
+  </si>
+  <si>
+    <t>Genuine Brother super high-yield (XXL Series) magenta ink for use in MFC-J4410dw, MFC-J4510dw, MFC-J4610dw, MFC-J4710dw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine Brother black high-yield ink cartridge for MFCJ4320DW, MFCJ4420DW, MFCJ4620DW, MFCJ5520DW and MFCJ5720DW. </t>
+  </si>
+  <si>
+    <t>Genuine Brother black super high-yield ink for MFCJ5520DW, MFCJ5620DW, MFCJ5720DW.</t>
+  </si>
+  <si>
+    <t>Genuine Brother super high-yield (XXL Series) cyan ink for use in MFC-J4410dw, MFC-J4510dw, MFC-J4610dw, MFC-J4710dw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine Brother cyan super high-yield ink cartridge for MFCJ4320DW, MFCJ4420DW, MFCJ4620DW, MFCJ5520DW and MFCJ5720DW. </t>
+  </si>
+  <si>
+    <t>Genuine Brother cyan XL ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-5910dw, MFC-J625dw, MFC-J6510dn, MFC-J6710dw, MFC-J6910dw, MFC-J825dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Genuine Brother Black XL ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-5910dw, MFC-J625dw, MFC-J6510dn, MFC-J6710dw, MFC-J6910dw, MFC-J825dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Genuine Brother yellow ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-J625dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Genuine Brother magenta ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-J625dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Premium compatible super high-yield XXL Series magenta ink for use in Brother MFC-J4410dw, MFC-J4510dw, MFC-J4610dw, MFC-J4710dw.</t>
+  </si>
+  <si>
+    <t>Genuine Brother super high-yield (XXL Series) yellow ink for use in MFC-J4410dw, MFC-J4510dw, MFC-J4610dw, MFC-J4710dw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium compatible yellow XL ink for Brother MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-5910dw, MFC-J625dw, MFC-J6510dn, MFC-J6710dw, MFC-J6910dw, MFC-J825dw, MFC-J835dw. Get OEM quality with the value that a trusted compatible toner offers. Formulated to resist fading, keeping text and images crisp. Each cartridge is tested prior to shipment to ensure your satisfaction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium compatible magenta XL ink for Brother MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-5910dw, MFC-J625dw, MFC-J6510dn, MFC-J6710dw, MFC-J6910dw, MFC-J825dw, MFC-J835dw. Get OEM quality with the value that a trusted compatible toner offers. Formulated to resist fading, keeping text and images crisp. Each cartridge is tested prior to shipment to ensure your satisfaction. </t>
+  </si>
+  <si>
+    <t>Genuine Brother black ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-J625dw, MFC-J825dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Genuine Brother cyan ink for MFC-J280w, MFC-J425w, MFC-J430w, MFC-J435w, MFC-J625dw, MFC-825dw, MFC-J835dw. Get the reliable OEM ink that will truly make a difference in your document.</t>
+  </si>
+  <si>
+    <t>Genuine Brother super high-yield (XXL Series) black ink for use in MFC-J4410dw, MFC-J4510dw, MFC-J4610dw, MFC-J4710dw. Contains 2 black LC107BK.</t>
+  </si>
+  <si>
+    <t>Genuine Brother black ultra high-yield ink cartridge for MFC-J6520DW, MFC-J6720DW, MFC-J6920DW.</t>
+  </si>
+  <si>
+    <t>Genuine Brother magenta ultra high-yield ink cartridge for MFC-J5830DW, MFC-J5930DW, MFC-J6535DW, MFC-J6935DW.</t>
+  </si>
+  <si>
+    <t>Genuine Brother black ink for MFC-J5910dw, MFC-J6510dw, MFC-J6710dw, MFC-J6910dw. Get the reliable OEM ink that will truly make a difference in your document quality. With rich black printing and clear grayscale reproduction, 'll appreciate the professional results on every page. Designed to maximize the efficiency of your machine.</t>
+  </si>
+  <si>
+    <t>Genuine Brother yellow ink for MFC-J5910dw, MFC-J6510dw, MFC-J6710dw, MFC-J6910dw. Get the reliable OEM ink that will truly make a difference in your document quality. With rich black printing and clear grayscale reproduction, 'll appreciate the professional results on every page. Designed to maximize the efficiency of your machine.</t>
+  </si>
+  <si>
+    <t>mfc-j870dw-656</t>
+  </si>
+  <si>
+    <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j870dw-656</t>
+  </si>
+  <si>
+    <t>mfc-j875dw-656</t>
+  </si>
+  <si>
+    <t>http://tonerprice.com/ink-toner/brother-ink-cartridges-toner/mfc/mfc-j875dw-656</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2817,8 +2956,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3096,389 +3236,678 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B459"/>
+  <dimension ref="A1:D459"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I415" sqref="I415"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>958</v>
+      </c>
+      <c r="D1" s="1">
+        <v>24.81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>957</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>955</v>
+      </c>
+      <c r="D3" s="1">
+        <v>46.14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>956</v>
+      </c>
+      <c r="D4" s="1">
+        <v>28.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>939</v>
+      </c>
+      <c r="D5" s="1">
+        <v>28.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>940</v>
+      </c>
+      <c r="D6" s="1">
+        <v>28.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>941</v>
+      </c>
+      <c r="D7" s="1">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>942</v>
+      </c>
+      <c r="D8" s="1">
+        <v>28.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>943</v>
+      </c>
+      <c r="D9" s="1">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>944</v>
+      </c>
+      <c r="D10" s="1">
+        <v>18.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>945</v>
+      </c>
+      <c r="D11" s="1">
+        <v>31.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>946</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>947</v>
+      </c>
+      <c r="D13" s="1">
+        <v>11.83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>948</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>949</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28.82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>950</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>951</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>952</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>953</v>
+      </c>
+      <c r="D19" s="1">
+        <v>11.83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>954</v>
+      </c>
+      <c r="D20" s="1">
+        <v>68.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>922</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>923</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45.89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>924</v>
+      </c>
+      <c r="D23" s="1">
+        <v>103.49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>925</v>
+      </c>
+      <c r="D24" s="1">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>926</v>
+      </c>
+      <c r="D25" s="1">
+        <v>89.62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>927</v>
+      </c>
+      <c r="D26" s="1">
+        <v>78.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>928</v>
+      </c>
+      <c r="D27" s="1">
+        <v>78.34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>929</v>
+      </c>
+      <c r="D28" s="1">
+        <v>520.55999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>930</v>
+      </c>
+      <c r="D29" s="1">
+        <v>51.73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>931</v>
+      </c>
+      <c r="D30" s="1">
+        <v>69.84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>932</v>
+      </c>
+      <c r="D31" s="1">
+        <v>51.73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>933</v>
+      </c>
+      <c r="D32" s="1">
+        <v>184.96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>64</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>934</v>
+      </c>
+      <c r="D33" s="1">
+        <v>206.94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>935</v>
+      </c>
+      <c r="D34" s="1">
+        <v>167.49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
       <c r="B35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>936</v>
+      </c>
+      <c r="D35" s="1">
+        <v>78.34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>937</v>
+      </c>
+      <c r="D36" s="1">
+        <v>31.94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
       <c r="B37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>938</v>
+      </c>
+      <c r="D37" s="1">
+        <v>80.92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
       <c r="B38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>915</v>
+      </c>
+      <c r="D38" s="1">
+        <v>178.76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>914</v>
+      </c>
+      <c r="D39" s="1">
+        <v>178.76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
       <c r="B40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>916</v>
+      </c>
+      <c r="D40" s="1">
+        <v>133.58000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
       <c r="B41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>915</v>
+      </c>
+      <c r="D41" s="1">
+        <v>95.73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>917</v>
+      </c>
+      <c r="D42" s="1">
+        <v>537.86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>916</v>
+      </c>
+      <c r="D43" s="1">
+        <v>83.56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>918</v>
+      </c>
+      <c r="D44" s="1">
+        <v>82.07</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>919</v>
+      </c>
+      <c r="D45" s="1">
+        <v>82.07</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
       <c r="B46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>920</v>
+      </c>
+      <c r="D46" s="1">
+        <v>38.340000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>92</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>921</v>
+      </c>
+      <c r="D47" s="1">
+        <v>368.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -6560,218 +6989,218 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>864</v>
+        <v>959</v>
       </c>
       <c r="B433" t="s">
-        <v>865</v>
+        <v>960</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B434" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>868</v>
+        <v>961</v>
       </c>
       <c r="B435" t="s">
-        <v>869</v>
+        <v>962</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B436" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="B437" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B438" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="B439" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="B440" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="B441" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B442" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="B443" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B444" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="B445" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B446" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="B447" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="B448" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="B449" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="B450" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="B451" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="B452" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="B453" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="B454" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="B455" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="B456" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="B457" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="B458" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="B459" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -6780,6 +7209,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>